<commit_message>
template change row height to see words
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\mfcworkstation\repos\JSRad\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\github\ECE-Radar-Project-Student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCFAC7-C343-48C3-B81B-C2A8AD56EB10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD10FCF5-795A-45B2-973E-E13FB042BC0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="K+gh3G7kKzmcTqDkG0hUn6d5jQaEfGLs6UlU+wsKe5eMvOWNQyImA7VZc9NPit4lUHAIAn2OOYywVkVmSJSE5Q==" workbookSaltValue="MPiuJGhpVmtRuUjL2odUDg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="21015" yWindow="180" windowWidth="24270" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27405" yWindow="5415" windowWidth="23250" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="87">
   <si>
     <t>Col0</t>
   </si>
@@ -625,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -716,6 +716,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,13 +1061,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="13" customWidth="1"/>
+    <col min="1" max="1" width="19.875" style="13" customWidth="1"/>
     <col min="2" max="4" width="12.5" style="13" customWidth="1"/>
     <col min="5" max="5" width="13.875" style="13" customWidth="1"/>
     <col min="6" max="10" width="12.5" style="13" customWidth="1"/>
@@ -1322,8 +1326,8 @@
       <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
+      <c r="B12" s="3">
+        <v>88.97</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
@@ -1357,8 +1361,8 @@
       <c r="B13" s="33">
         <v>235.39333530158299</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
+      <c r="C13" s="3">
+        <v>622.79</v>
       </c>
       <c r="D13" s="33">
         <v>911.67446743124935</v>
@@ -1899,23 +1903,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="40" t="s">
         <v>35</v>
       </c>
       <c r="G32" s="13" t="s">
@@ -4532,11 +4536,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mhFSh7uS33s4wCaqKXllMuFTZhA4xkhZCQXGUefc0zsVn60xgoV/zH29t2f73aJmq9PXY0x3jaUxGWf2HdFthg==" saltValue="9tWDMbIXAtC8lXzuy9WrcA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="VA6vgcd4lZ1xSykf9woA9nci5P62h25IVhEfuDsKuPVKe1taB1yR8h8W2Lk20DIoY1ppEEbn4nCLNk3ww/VRcA==" saltValue="YBqGr64pfkU42XQyxk9fdw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J1 A9:J9 A2 D2 A11:J13 A10 A17:J17 A16 A32:J37 A31 A39:J43 A38 A45:J51 A44 A53:J59 A52 A61:J65 A60 A67:J71 A66 A73:J92 A72 A94:J99 A93 A101:J120 A100 A3:D3 A4:A5 A6:A8 D4:D5 D6:D8 A19:J30 A18:C18 E18:J18 A15:J15 A14:F14 H14:J14" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J1 A9:J9 A2 D2 A11:J11 A10 A17:J17 A16 A32:J37 A31 A39:J43 A38 A45:J51 A44 A53:J59 A52 A61:J65 A60 A67:J71 A66 A73:J92 A72 A94:J99 A93 A101:J120 A100 A3:D3 A4:A5 A6:A8 D4:D5 D6:D8 A19:J30 A18:C18 E18:J18 A15:J15 A14:F14 H14:J14 A13:B13 A12 C12:J12 D13:J13" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4638,21 +4642,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002150F9E13E4DB341AD798B7DFE367926" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbf7242a78008123cee6a1ecd6703a48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2f7f3735-0479-41e9-b500-9d501c7e9a5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="623bc7ee9fc1715608191026e55b1d41" ns2:_="">
     <xsd:import namespace="2f7f3735-0479-41e9-b500-9d501c7e9a5a"/>
@@ -4830,24 +4819,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79C03B55-D523-4788-B95C-60A9432DBAB0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC69F735-ECA1-4382-BFED-67EB87D29AA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12A3834E-F750-42DA-843D-53E394C7C9A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4863,4 +4850,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79C03B55-D523-4788-B95C-60A9432DBAB0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC69F735-ECA1-4382-BFED-67EB87D29AA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>